<commit_message>
fiinally validated all the outcomes. The code is in ctn0094_data_gabriel/, but now that they are correct I'll be moving them into vignettes here.
</commit_message>
<xml_diff>
--- a/inst/suppl_docs/definitions_20220210.xlsx
+++ b/inst/suppl_docs/definitions_20220210.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\godom\GitHub\CTN-0094\CTNote\inst\suppl_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielodom/Documents/GitHub/CTN-0094/CTNote/inst/suppl_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0800FA8-5410-4829-A838-BD85BF30CE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CE0E39-7596-4844-A202-725F5B55CF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E30E9EF-9AAA-CD48-B338-97B5233CAF9E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{5E30E9EF-9AAA-CD48-B338-97B5233CAF9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="205">
   <si>
     <t>Primary Endpoint</t>
   </si>
@@ -1051,22 +1051,13 @@
     <t>DROP</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Fiellin et al., 2006; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Krupitsky et al., 2011</t>
-    </r>
-  </si>
-  <si>
-    <t>Should Krupitsky have a week 5-24 window?</t>
+    <t>weekly from weeks 5-24</t>
+  </si>
+  <si>
+    <t>DROP (b)</t>
+  </si>
+  <si>
+    <t>Apply Matick 2003 (A)</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +1271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1331,6 +1322,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1646,24 +1640,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1123D4-B217-1541-959A-BB4DAF6F68A4}">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.375" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
-    <col min="5" max="5" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.875" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
     <col min="8" max="8" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="46" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>135</v>
       </c>
@@ -1692,7 +1686,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
@@ -1718,7 +1712,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
@@ -1744,7 +1738,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
@@ -1770,7 +1764,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="47" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
@@ -1796,7 +1790,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
@@ -1822,7 +1816,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>5</v>
       </c>
@@ -1848,7 +1842,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>5</v>
       </c>
@@ -1874,7 +1868,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="116.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>5</v>
       </c>
@@ -1900,7 +1894,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="57" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>5</v>
       </c>
@@ -1929,7 +1923,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="204" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>5</v>
       </c>
@@ -1955,7 +1949,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>5</v>
       </c>
@@ -1966,7 +1960,7 @@
         <v>143</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>202</v>
+        <v>104</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>38</v>
@@ -1980,89 +1974,88 @@
       <c r="H12" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="I12" s="17" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14" spans="1:9" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H14" s="15" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H15" s="15" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="130.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="57" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>42</v>
       </c>
@@ -2073,126 +2066,129 @@
         <v>138</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="H18" s="15" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
+    <row r="19" spans="1:9" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B19" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="H19" s="15" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="4" t="s">
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="H20" s="15" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="I20" s="17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>57</v>
       </c>
@@ -2200,25 +2196,25 @@
         <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>57</v>
       </c>
@@ -2226,25 +2222,25 @@
         <v>58</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="30.75" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>57</v>
       </c>
@@ -2255,22 +2251,22 @@
         <v>141</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>161</v>
+        <v>68</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>163</v>
+        <v>10</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="31" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
         <v>57</v>
       </c>
@@ -2281,22 +2277,22 @@
         <v>141</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>71</v>
+        <v>161</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>73</v>
+        <v>163</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>57</v>
       </c>
@@ -2307,22 +2303,22 @@
         <v>141</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>57</v>
       </c>
@@ -2333,22 +2329,22 @@
         <v>141</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
         <v>57</v>
       </c>
@@ -2356,25 +2352,25 @@
         <v>58</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>53</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="85.5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>57</v>
       </c>
@@ -2382,25 +2378,25 @@
         <v>58</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>168</v>
+        <v>80</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="90" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
         <v>57</v>
       </c>
@@ -2411,22 +2407,25 @@
         <v>141</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>83</v>
+        <v>168</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
         <v>57</v>
       </c>
@@ -2436,23 +2435,23 @@
       <c r="C30" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>86</v>
+      <c r="D30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
         <v>57</v>
       </c>
@@ -2460,25 +2459,25 @@
         <v>58</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>53</v>
+        <v>141</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
         <v>57</v>
       </c>
@@ -2486,25 +2485,25 @@
         <v>58</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>10</v>
+        <v>173</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>57</v>
       </c>
@@ -2512,103 +2511,103 @@
         <v>58</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="15" t="s">
+      <c r="H34" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
         <v>57</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="2" t="s">
         <v>137</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>12</v>
+        <v>97</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="13" t="s">
         <v>57</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>141</v>
+      <c r="C36" s="17" t="s">
+        <v>137</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="187.5" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
         <v>57</v>
       </c>
@@ -2619,22 +2618,22 @@
         <v>141</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>176</v>
+        <v>101</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="120" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
         <v>57</v>
       </c>
@@ -2645,22 +2644,22 @@
         <v>141</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>105</v>
+        <v>176</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
         <v>57</v>
       </c>
@@ -2668,13 +2667,13 @@
         <v>94</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>12</v>
@@ -2683,10 +2682,10 @@
         <v>16</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
         <v>57</v>
       </c>
@@ -2694,13 +2693,13 @@
         <v>94</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>12</v>
@@ -2709,10 +2708,13 @@
         <v>16</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="204" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="I40" s="19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
         <v>57</v>
       </c>
@@ -2723,22 +2725,22 @@
         <v>141</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>111</v>
+        <v>12</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="116.25" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
         <v>57</v>
       </c>
@@ -2749,22 +2751,22 @@
         <v>141</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>112</v>
+        <v>35</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
         <v>57</v>
       </c>
@@ -2775,22 +2777,22 @@
         <v>141</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>16</v>
+        <v>114</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
         <v>57</v>
       </c>
@@ -2798,25 +2800,25 @@
         <v>94</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
         <v>57</v>
       </c>
@@ -2824,25 +2826,25 @@
         <v>94</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>121</v>
+        <v>9</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
         <v>57</v>
       </c>
@@ -2850,25 +2852,25 @@
         <v>94</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>10</v>
+      <c r="G46" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="75" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
         <v>57</v>
       </c>
@@ -2876,25 +2878,25 @@
         <v>94</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>7</v>
+        <v>122</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>187</v>
+        <v>123</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
         <v>57</v>
       </c>
@@ -2902,13 +2904,13 @@
         <v>94</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>9</v>
@@ -2917,10 +2919,10 @@
         <v>10</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="114" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
         <v>57</v>
       </c>
@@ -2928,25 +2930,25 @@
         <v>94</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>124</v>
+        <v>7</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="120" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>57</v>
       </c>
@@ -2957,22 +2959,22 @@
         <v>141</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>126</v>
+        <v>191</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="s">
         <v>57</v>
       </c>
@@ -2983,22 +2985,22 @@
         <v>141</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>26</v>
+        <v>125</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="13" t="s">
         <v>57</v>
       </c>
@@ -3009,10 +3011,10 @@
         <v>141</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>128</v>
+        <v>26</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>9</v>
@@ -3021,10 +3023,10 @@
         <v>28</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
         <v>57</v>
       </c>
@@ -3035,22 +3037,22 @@
         <v>141</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>131</v>
+        <v>28</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
         <v>57</v>
       </c>
@@ -3061,18 +3063,44 @@
         <v>141</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G54" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A55" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G55" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H54" s="16" t="s">
+      <c r="H55" s="16" t="s">
         <v>197</v>
       </c>
     </row>

</xml_diff>